<commit_message>
Added colors to site.css file.
</commit_message>
<xml_diff>
--- a/Documents/Database/DatabaseTables.xlsx
+++ b/Documents/Database/DatabaseTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregw\source\repos\OLLLibrarySystem\Documents\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4740B854-F311-447C-B88A-1220AEEE6B75}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EDECE6-C435-4EC8-8EAE-DE76459B645E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{EB657813-76F0-4FB0-96CD-6C8B36318B17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" xr2:uid="{EB657813-76F0-4FB0-96CD-6C8B36318B17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,33 +424,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,13 +461,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,208 +812,208 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="13"/>
-      <c r="F2" s="3" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="28"/>
+      <c r="F2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="3" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="28"/>
+      <c r="J2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="13"/>
-      <c r="N2" s="20" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="28"/>
+      <c r="N2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
-      <c r="R2" s="3" t="s">
+      <c r="O2" s="26"/>
+      <c r="P2" s="27"/>
+      <c r="R2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="5"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="24"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="11" t="s">
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="23" t="s">
+      <c r="L3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="11" t="s">
+      <c r="P3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="D4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15" t="s">
+      <c r="H4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27" t="s">
+      <c r="N4" s="18"/>
+      <c r="O4" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" s="11"/>
-      <c r="S4" s="12" t="s">
+      <c r="P4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="7"/>
+      <c r="S4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T4" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="14" t="s">
+      <c r="D5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15" t="s">
+      <c r="H5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24" t="s">
+      <c r="N5" s="15"/>
+      <c r="O5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="P5" s="21" t="s">
         <v>45</v>
       </c>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="D6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15" t="s">
+      <c r="H6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="14" t="s">
+      <c r="D7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="H7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="6" t="s">
         <v>37</v>
       </c>
       <c r="O7" t="s">
@@ -1021,20 +1021,20 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="19" t="s">
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="11" t="s">
         <v>40</v>
       </c>
       <c r="O8" t="s">
@@ -1042,241 +1042,241 @@
       </c>
     </row>
     <row r="9" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="28"/>
       <c r="O9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="19" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="19" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="6" t="s">
+      <c r="J12" s="7"/>
+      <c r="K12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="13"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="28"/>
     </row>
     <row r="15" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="13"/>
-      <c r="N15" s="11" t="s">
+      <c r="K15" s="23"/>
+      <c r="L15" s="28"/>
+      <c r="N15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="12" t="s">
+      <c r="O15" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="P15" s="8" t="s">
+      <c r="P15" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N16" s="11"/>
-      <c r="O16" s="12" t="s">
+      <c r="L16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="8" t="s">
+      <c r="P16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="6:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="12" t="s">
+      <c r="G17" s="29"/>
+      <c r="H17" s="24"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="11" t="s">
+      <c r="L17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O17" s="12" t="s">
+      <c r="O17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F19" s="6"/>
-      <c r="G19" s="6" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="6" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J15:L15"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="N14:P14"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>